<commit_message>
add more elements in the dayahead...
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="说明" sheetId="4" r:id="rId1"/>
@@ -14375,7 +14375,7 @@
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B3" sqref="B3:Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14928,10 +14928,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14972,16 +14972,16 @@
         <v>16</v>
       </c>
       <c r="C3" s="2">
-        <v>1500</v>
+        <v>800</v>
       </c>
       <c r="D3" s="2">
-        <v>3000</v>
+        <v>1600</v>
       </c>
       <c r="E3" s="2">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="F3" s="2">
-        <v>-400</v>
+        <v>-200</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -14991,6 +14991,78 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>11</v>
+      </c>
+      <c r="N4">
+        <v>12</v>
+      </c>
+      <c r="O4">
+        <v>13</v>
+      </c>
+      <c r="P4">
+        <v>14</v>
+      </c>
+      <c r="Q4">
+        <v>15</v>
+      </c>
+      <c r="R4">
+        <v>16</v>
+      </c>
+      <c r="S4">
+        <v>17</v>
+      </c>
+      <c r="T4">
+        <v>18</v>
+      </c>
+      <c r="U4">
+        <v>19</v>
+      </c>
+      <c r="V4">
+        <v>20</v>
+      </c>
+      <c r="W4">
+        <v>21</v>
+      </c>
+      <c r="X4">
+        <v>22</v>
+      </c>
+      <c r="Y4">
+        <v>23</v>
+      </c>
+      <c r="Z4">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5">
@@ -15790,6 +15862,80 @@
       </c>
       <c r="Z14">
         <v>3.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="C16">
+        <v>1.7</v>
+      </c>
+      <c r="D16">
+        <v>1.4</v>
+      </c>
+      <c r="E16">
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="F16">
+        <v>1.6</v>
+      </c>
+      <c r="G16">
+        <v>1.6</v>
+      </c>
+      <c r="H16">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="I16">
+        <v>1.9</v>
+      </c>
+      <c r="J16">
+        <v>2.1</v>
+      </c>
+      <c r="K16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L16">
+        <v>2.1</v>
+      </c>
+      <c r="M16">
+        <v>2.1</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>1.9</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="R16">
+        <v>1.9</v>
+      </c>
+      <c r="S16">
+        <v>2.1</v>
+      </c>
+      <c r="T16">
+        <v>3</v>
+      </c>
+      <c r="U16">
+        <v>2.5</v>
+      </c>
+      <c r="V16">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="W16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X16">
+        <v>2.5</v>
+      </c>
+      <c r="Y16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Z16">
+        <v>1.7000000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -17761,7 +17907,7 @@
       <c r="B20" s="10"/>
       <c r="C20" s="4">
         <f ca="1">(C$15+RAND()*1000+_xlfn.GAUSS(RAND()*2-1)*1000)/500</f>
-        <v>3.7863526105811465</v>
+        <v>4.5231139475915079</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -17774,14 +17920,14 @@
       <c r="B23" s="10"/>
       <c r="T23" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>0.14506940133419688</v>
+        <v>-0.25521940517501068</v>
       </c>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="10"/>
       <c r="T24" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>0.14433840697087308</v>
+        <v>0.27815892595291236</v>
       </c>
     </row>
     <row r="25" spans="2:20">
@@ -17795,14 +17941,14 @@
       <c r="B26" s="10"/>
       <c r="T26" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>0.16555527955814398</v>
+        <v>-0.33991098509829198</v>
       </c>
     </row>
     <row r="27" spans="2:20">
       <c r="B27" s="10"/>
       <c r="T27" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>5.2419106349185007E-2</v>
+        <v>0.27897725522114825</v>
       </c>
     </row>
   </sheetData>
@@ -18832,7 +18978,7 @@
       <c r="B20" s="10"/>
       <c r="C20" s="4">
         <f ca="1">(C$15+RAND()*1000+_xlfn.GAUSS(RAND()*2-1)*1000)/500</f>
-        <v>1.2717458219656257</v>
+        <v>1.9717458201354379</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -18845,14 +18991,14 @@
       <c r="B23" s="10"/>
       <c r="T23" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>7.8591798154733716E-2</v>
+        <v>0.10394668195842871</v>
       </c>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="10"/>
       <c r="T24" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>-0.32225124944127026</v>
+        <v>-0.21498538376941212</v>
       </c>
     </row>
     <row r="25" spans="2:20">
@@ -18866,14 +19012,14 @@
       <c r="B26" s="10"/>
       <c r="T26" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>0.27826669219401012</v>
+        <v>-0.19327817761411725</v>
       </c>
     </row>
     <row r="27" spans="2:20">
       <c r="B27" s="10"/>
       <c r="T27" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>8.0719223806072327E-2</v>
+        <v>-0.21680205856442147</v>
       </c>
     </row>
   </sheetData>
@@ -19902,7 +20048,7 @@
       <c r="B20" s="10"/>
       <c r="C20" s="4">
         <f ca="1">C$15/100*((RAND()*2-1)*0.1+_xlfn.GAUSS(RAND()*2-1)*0.1+1)+(RAND()*2-1)+_xlfn.GAUSS(RAND()*2-1)+1</f>
-        <v>6.6366048672202158</v>
+        <v>5.7996223038677783</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -20957,7 +21103,7 @@
       <c r="B20" s="10"/>
       <c r="C20" s="4">
         <f ca="1">C$15/100*((RAND()*2-1)*0.1+_xlfn.GAUSS(RAND()*2-1)*0.1+1)+(RAND()*2-1)+_xlfn.GAUSS(RAND()*2-1)*4</f>
-        <v>4.8537419689305219</v>
+        <v>3.7929031141139604</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -20970,14 +21116,14 @@
       <c r="B23" s="10"/>
       <c r="T23" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>0.14799283993275869</v>
+        <v>0.29673949072446215</v>
       </c>
     </row>
     <row r="24" spans="2:20">
       <c r="B24" s="10"/>
       <c r="T24" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>-0.11388800192429344</v>
+        <v>0.2618263854030809</v>
       </c>
     </row>
     <row r="25" spans="2:20">
@@ -20991,14 +21137,14 @@
       <c r="B26" s="10"/>
       <c r="T26" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>-0.30116904897657809</v>
+        <v>-0.26924764766339759</v>
       </c>
     </row>
     <row r="27" spans="2:20">
       <c r="B27" s="10"/>
       <c r="T27" s="8">
         <f ca="1">_xlfn.GAUSS(RAND()*2-1)</f>
-        <v>-0.23342266618689578</v>
+        <v>-0.33329520881645464</v>
       </c>
     </row>
   </sheetData>
@@ -22027,7 +22173,7 @@
       <c r="B20" s="10"/>
       <c r="C20" s="4">
         <f ca="1">C$15/500*((RAND()*2-1)*0.1+_xlfn.GAUSS(RAND()*2-1)*0.1+1)+(RAND()*2-1)+_xlfn.GAUSS(RAND()*2-1)*2</f>
-        <v>5.2885306807922277</v>
+        <v>5.4644169211421065</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -22067,7 +22213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Z27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -23082,7 +23228,7 @@
       <c r="B20" s="10"/>
       <c r="C20" s="4">
         <f ca="1">C$15/400*((RAND()*2-1)*0.1+_xlfn.GAUSS(RAND()*2-1)*0.1+1)+(RAND()*2-1)+_xlfn.GAUSS(RAND()*2-1)*2</f>
-        <v>5.4992702289337263</v>
+        <v>4.0347237603005901</v>
       </c>
     </row>
     <row r="21" spans="2:20">

</xml_diff>